<commit_message>
überarbeitet für eine bessere Darstellung
</commit_message>
<xml_diff>
--- a/src/main/resources/document/Wetterstationen.xlsx
+++ b/src/main/resources/document/Wetterstationen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAG\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAG\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD10BCD9-E191-4FB1-A3A4-D163A82C8700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBCB957-75F9-46B2-9A06-5BD4E9A6F50E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="14910" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="525" windowWidth="28320" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -530,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,18 +757,18 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>